<commit_message>
small improvements, add GPIOs to excel
</commit_message>
<xml_diff>
--- a/SHEEP TEST PINS.xlsx
+++ b/SHEEP TEST PINS.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oliver/Desktop/SHEEP TESTER/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oliver/Documents/GitHub/sheep-tester/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D2478A0-9DFE-9747-B33C-85BA828A4E35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26078C0E-580A-8441-9FD4-B1DD3AC685DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="680" windowWidth="34500" windowHeight="19900" xr2:uid="{251F4D23-F6BB-8045-A7D4-E73691D00F1E}"/>
+    <workbookView xWindow="34560" yWindow="-14000" windowWidth="51200" windowHeight="20980" xr2:uid="{251F4D23-F6BB-8045-A7D4-E73691D00F1E}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="187">
   <si>
     <t>TP1</t>
   </si>
@@ -295,12 +295,6 @@
     <t>check if LED signal comes out</t>
   </si>
   <si>
-    <t>*Rpi fast enough? Should we add a LED and measure the brightness/color?</t>
-  </si>
-  <si>
-    <t>*Rpi fast enough? Can we use ESP32 to test itself?</t>
-  </si>
-  <si>
     <t>GPIO32</t>
   </si>
   <si>
@@ -310,12 +304,6 @@
     <t>PoE injection test</t>
   </si>
   <si>
-    <t>MD1 pin</t>
-  </si>
-  <si>
-    <t>J9 pin</t>
-  </si>
-  <si>
     <t>GPIO16 / U1TXD</t>
   </si>
   <si>
@@ -328,18 +316,12 @@
     <t>read the QR code</t>
   </si>
   <si>
-    <t>*</t>
-  </si>
-  <si>
     <t>TP-Link TL-SG1005LP, switchable LAN connection</t>
   </si>
   <si>
     <t>usb qr code scanner</t>
   </si>
   <si>
-    <t>result output</t>
-  </si>
-  <si>
     <t>RPI pin</t>
   </si>
   <si>
@@ -373,14 +355,254 @@
     <t>OC output at pi pullup at pi, ESP signal feedback through serial connection</t>
   </si>
   <si>
-    <t>7 segment + LEDs</t>
+    <t>Signals</t>
+  </si>
+  <si>
+    <t>#GPIO12</t>
+  </si>
+  <si>
+    <t>AIN0_U4</t>
+  </si>
+  <si>
+    <t>AIN1_U4</t>
+  </si>
+  <si>
+    <t>B0_U2</t>
+  </si>
+  <si>
+    <t>B1_U2</t>
+  </si>
+  <si>
+    <t>AIN2_U4</t>
+  </si>
+  <si>
+    <t>AIN3_U4</t>
+  </si>
+  <si>
+    <t>AIN0_U5</t>
+  </si>
+  <si>
+    <t>AIN1_U5</t>
+  </si>
+  <si>
+    <t>AIN2_U5</t>
+  </si>
+  <si>
+    <t>AIN3_U5</t>
+  </si>
+  <si>
+    <t>AIN0_U6</t>
+  </si>
+  <si>
+    <t>AIN1_U6</t>
+  </si>
+  <si>
+    <t>AIN2_U6</t>
+  </si>
+  <si>
+    <t>AIN3_U6</t>
+  </si>
+  <si>
+    <t>AIN0_U7</t>
+  </si>
+  <si>
+    <t>B5_U2_U12 = 60V / #12V preselect, B3_U2 = 60V, B4_U2 = 12V</t>
+  </si>
+  <si>
+    <t>B6_U3</t>
+  </si>
+  <si>
+    <t>B2_U2</t>
+  </si>
+  <si>
+    <t>B6_U2</t>
+  </si>
+  <si>
+    <t>A3_U2</t>
+  </si>
+  <si>
+    <t>relays = A7_U2_U12</t>
+  </si>
+  <si>
+    <t>B0_U3_U12</t>
+  </si>
+  <si>
+    <t>A6_U2_U12</t>
+  </si>
+  <si>
+    <t>relay = B4_U3_U12</t>
+  </si>
+  <si>
+    <t>GPIO13</t>
+  </si>
+  <si>
+    <t>A2_U2</t>
+  </si>
+  <si>
+    <t>A0_U2</t>
+  </si>
+  <si>
+    <t>A1_U2</t>
+  </si>
+  <si>
+    <t>B7_U2</t>
+  </si>
+  <si>
+    <t>A4_U2</t>
+  </si>
+  <si>
+    <t>A5_U2</t>
+  </si>
+  <si>
+    <t>TP_GPIO32</t>
+  </si>
+  <si>
+    <t>TP_GPIO16</t>
+  </si>
+  <si>
+    <t>TP_GPIO36</t>
+  </si>
+  <si>
+    <t>B1_U3</t>
+  </si>
+  <si>
+    <t>B2_U3</t>
+  </si>
+  <si>
+    <t>B3_U3</t>
+  </si>
+  <si>
+    <t>B5_U3_U12</t>
+  </si>
+  <si>
+    <t>shutdown button</t>
+  </si>
+  <si>
+    <t>GPIO26</t>
+  </si>
+  <si>
+    <t>GPIO20</t>
+  </si>
+  <si>
+    <t>GPIO21</t>
+  </si>
+  <si>
+    <t>LED GOOD</t>
+  </si>
+  <si>
+    <t>LED BAD</t>
+  </si>
+  <si>
+    <t>7SEG_A_0</t>
+  </si>
+  <si>
+    <t>7SEG_B_0</t>
+  </si>
+  <si>
+    <t>7SEG_C_0</t>
+  </si>
+  <si>
+    <t>7SEG_D_0</t>
+  </si>
+  <si>
+    <t>7SEG_E_0</t>
+  </si>
+  <si>
+    <t>7SEG_F_0</t>
+  </si>
+  <si>
+    <t>7SEG_G_0</t>
+  </si>
+  <si>
+    <t>7SEG_A_1</t>
+  </si>
+  <si>
+    <t>7SEG_B_1</t>
+  </si>
+  <si>
+    <t>7SEG_C_1</t>
+  </si>
+  <si>
+    <t>7SEG_D_1</t>
+  </si>
+  <si>
+    <t>7SEG_E_1</t>
+  </si>
+  <si>
+    <t>7SEG_F_1</t>
+  </si>
+  <si>
+    <t>7SEG_G_1</t>
+  </si>
+  <si>
+    <t>GPIO17</t>
+  </si>
+  <si>
+    <t>GPIO18</t>
+  </si>
+  <si>
+    <t>GPIO27</t>
+  </si>
+  <si>
+    <t>GPIO22</t>
+  </si>
+  <si>
+    <t>GPIO23</t>
+  </si>
+  <si>
+    <t>GPIO24</t>
+  </si>
+  <si>
+    <t>GPIO10</t>
+  </si>
+  <si>
+    <t>GPIO25</t>
+  </si>
+  <si>
+    <t>GPIO9</t>
+  </si>
+  <si>
+    <t>GPIO8</t>
+  </si>
+  <si>
+    <t>GPIO11</t>
+  </si>
+  <si>
+    <t>GPIO7</t>
+  </si>
+  <si>
+    <t>GPIO19</t>
+  </si>
+  <si>
+    <t>GPIO16</t>
+  </si>
+  <si>
+    <t>MCP23017_#RESET</t>
+  </si>
+  <si>
+    <t>GPIO4</t>
+  </si>
+  <si>
+    <t>SDA</t>
+  </si>
+  <si>
+    <t>SCL</t>
+  </si>
+  <si>
+    <t>GPIO2</t>
+  </si>
+  <si>
+    <t>GPIO3</t>
+  </si>
+  <si>
+    <t>I2C</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -401,6 +623,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -411,7 +639,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -428,10 +656,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -746,51 +975,56 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{715C4E4B-8507-464D-BE22-772D7378D4BF}">
-  <dimension ref="A1:J47"/>
+  <dimension ref="A1:J53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C47" sqref="C47"/>
+    <sheetView tabSelected="1" zoomScale="117" zoomScaleNormal="117" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="21.5" customWidth="1"/>
     <col min="3" max="3" width="51.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="98.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="32.1640625" customWidth="1"/>
+    <col min="4" max="4" width="78" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" customWidth="1"/>
+    <col min="6" max="6" width="32.1640625" customWidth="1"/>
+    <col min="7" max="7" width="55.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="E1" t="s">
-        <v>101</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="E1" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" s="3" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -801,17 +1035,13 @@
         <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -824,15 +1054,11 @@
       <c r="D3" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1">
-        <v>1</v>
-      </c>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-    </row>
-    <row r="4" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H3" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -845,11 +1071,11 @@
       <c r="D4" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="H4" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I4" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -862,14 +1088,14 @@
       <c r="D5" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="F5" s="1">
-        <v>1</v>
-      </c>
-      <c r="H5" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="G5" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -882,14 +1108,14 @@
       <c r="D6" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="F6" s="1">
-        <v>1</v>
-      </c>
-      <c r="H6" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="G6" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -900,16 +1126,16 @@
         <v>64</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="F7" s="1">
-        <v>3</v>
-      </c>
-      <c r="H7" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+        <v>100</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -920,16 +1146,16 @@
         <v>66</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="F8" s="1">
-        <v>1</v>
-      </c>
-      <c r="H8" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -942,11 +1168,11 @@
       <c r="D9" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="H9" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I9" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -959,11 +1185,11 @@
       <c r="D10" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="H10" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I10" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -976,14 +1202,14 @@
       <c r="D11" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="F11" s="1">
-        <v>1</v>
-      </c>
-      <c r="H11" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="G11" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -994,13 +1220,13 @@
         <v>71</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="F12" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+        <v>103</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -1011,13 +1237,13 @@
         <v>71</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="F13" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+        <v>103</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
@@ -1030,11 +1256,14 @@
       <c r="D14" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="E14" s="2" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F14" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
@@ -1047,11 +1276,11 @@
       <c r="D15" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="E15" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F15" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
@@ -1064,14 +1293,11 @@
       <c r="D16" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="E16" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="G16" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F16" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
@@ -1084,11 +1310,11 @@
       <c r="D17" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="E17" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F17" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
@@ -1099,13 +1325,13 @@
         <v>74</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="F18" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+        <v>104</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
@@ -1118,11 +1344,11 @@
       <c r="D19" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="F19" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="G19" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
@@ -1135,11 +1361,11 @@
       <c r="D20" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="H20" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I20" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
@@ -1152,17 +1378,17 @@
       <c r="D21" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="F21" s="1">
-        <v>1</v>
-      </c>
-      <c r="G21" s="1">
-        <v>1</v>
-      </c>
-      <c r="H21" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="G21" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
@@ -1175,17 +1401,17 @@
       <c r="D22" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="F22" s="1">
-        <v>1</v>
-      </c>
-      <c r="G22" s="1">
-        <v>1</v>
-      </c>
-      <c r="H22" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="G22" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
@@ -1198,14 +1424,14 @@
       <c r="D23" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="F23" s="1">
-        <v>1</v>
-      </c>
-      <c r="H23" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="G23" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
@@ -1218,17 +1444,14 @@
       <c r="D24" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="F24" s="1">
-        <v>1</v>
-      </c>
-      <c r="H24" s="1">
-        <v>1</v>
-      </c>
-      <c r="J24" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="G24" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
@@ -1241,119 +1464,250 @@
       <c r="D25" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="G25" s="1">
-        <v>1</v>
-      </c>
-      <c r="J25" s="1" t="s">
+      <c r="G25" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
+      <c r="C27" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B31" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B32" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B30" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="G30" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
+      <c r="C32" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B31" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="G31" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B32" s="1" t="s">
+      <c r="D32" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="C32" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="G32" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="33" spans="2:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B33" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B34" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B35" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="F35" s="1">
-        <v>1</v>
-      </c>
-      <c r="J35" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="39" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+        <v>151</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B36" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B37" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B38" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B39" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="42" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+        <v>155</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B40" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B41" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="42" spans="2:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B42" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="47" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="F47">
-        <f>SUM(F2:F46)</f>
-        <v>16</v>
-      </c>
-      <c r="G47">
-        <f t="shared" ref="G47:I47" si="0">SUM(G2:G46)</f>
-        <v>8</v>
-      </c>
-      <c r="H47">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="I47">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <v>158</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B43" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B44" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B45" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B46" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="47" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B47" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="48" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B48" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="49" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B49" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="51" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B51" t="s">
+        <v>180</v>
+      </c>
+      <c r="G51" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="52" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B52" t="s">
+        <v>182</v>
+      </c>
+      <c r="G52" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="53" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B53" t="s">
+        <v>183</v>
+      </c>
+      <c r="G53" t="s">
+        <v>185</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
correct GPIOs in excel
</commit_message>
<xml_diff>
--- a/SHEEP TEST PINS.xlsx
+++ b/SHEEP TEST PINS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11122"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oliver/Documents/GitHub/sheep-tester/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26078C0E-580A-8441-9FD4-B1DD3AC685DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83889645-A288-6F45-A72C-CA399ED89C4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34560" yWindow="-14000" windowWidth="51200" windowHeight="20980" xr2:uid="{251F4D23-F6BB-8045-A7D4-E73691D00F1E}"/>
+    <workbookView xWindow="0" yWindow="620" windowWidth="28800" windowHeight="16300" xr2:uid="{251F4D23-F6BB-8045-A7D4-E73691D00F1E}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -151,9 +151,6 @@
     <t>SMOKE signal</t>
   </si>
   <si>
-    <t>SMOKE signal divided</t>
-  </si>
-  <si>
     <t>beeper, cathode</t>
   </si>
   <si>
@@ -295,9 +292,6 @@
     <t>check if LED signal comes out</t>
   </si>
   <si>
-    <t>GPIO32</t>
-  </si>
-  <si>
     <t>PoE</t>
   </si>
   <si>
@@ -454,9 +448,6 @@
     <t>A5_U2</t>
   </si>
   <si>
-    <t>TP_GPIO32</t>
-  </si>
-  <si>
     <t>TP_GPIO16</t>
   </si>
   <si>
@@ -596,6 +587,15 @@
   </si>
   <si>
     <t>I2C</t>
+  </si>
+  <si>
+    <t>GPIO35</t>
+  </si>
+  <si>
+    <t>TP_GPIO35</t>
+  </si>
+  <si>
+    <t>GPI34 / SMOKE signal divided</t>
   </si>
 </sst>
 </file>
@@ -656,10 +656,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -978,736 +977,733 @@
   <dimension ref="A1:J53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="117" zoomScaleNormal="117" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C33" sqref="C33"/>
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="21.5" customWidth="1"/>
+    <col min="2" max="2" width="25.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="51.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="78" customWidth="1"/>
+    <col min="4" max="4" width="75.33203125" customWidth="1"/>
     <col min="5" max="5" width="10.6640625" customWidth="1"/>
     <col min="6" max="6" width="32.1640625" customWidth="1"/>
     <col min="7" max="7" width="55.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>100</v>
+      </c>
+      <c r="J2" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
         <v>49</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D4" t="s">
         <v>53</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="I4" t="s">
         <v>106</v>
       </c>
-      <c r="F1" s="3" t="s">
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D5" t="s">
+        <v>54</v>
+      </c>
+      <c r="G5" t="s">
+        <v>108</v>
+      </c>
+      <c r="I5" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" t="s">
+        <v>58</v>
+      </c>
+      <c r="D6" t="s">
+        <v>60</v>
+      </c>
+      <c r="G6" t="s">
+        <v>109</v>
+      </c>
+      <c r="I6" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" t="s">
+        <v>63</v>
+      </c>
+      <c r="D7" t="s">
+        <v>98</v>
+      </c>
+      <c r="G7" t="s">
+        <v>121</v>
+      </c>
+      <c r="I7" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" t="s">
+        <v>65</v>
+      </c>
+      <c r="D8" t="s">
+        <v>99</v>
+      </c>
+      <c r="G8" t="s">
+        <v>122</v>
+      </c>
+      <c r="I8" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D9" t="s">
+        <v>66</v>
+      </c>
+      <c r="I9" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D10" t="s">
+        <v>69</v>
+      </c>
+      <c r="I10" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" t="s">
+        <v>61</v>
+      </c>
+      <c r="D11" t="s">
+        <v>62</v>
+      </c>
+      <c r="G11" t="s">
+        <v>123</v>
+      </c>
+      <c r="I11" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" t="s">
+        <v>70</v>
+      </c>
+      <c r="D12" t="s">
+        <v>101</v>
+      </c>
+      <c r="G12" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" t="s">
+        <v>70</v>
+      </c>
+      <c r="D13" t="s">
+        <v>101</v>
+      </c>
+      <c r="G13" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" t="s">
+        <v>71</v>
+      </c>
+      <c r="D14" t="s">
+        <v>72</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="G14" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" t="s">
+        <v>71</v>
+      </c>
+      <c r="D15" t="s">
+        <v>72</v>
+      </c>
+      <c r="F15" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" t="s">
+        <v>71</v>
+      </c>
+      <c r="D16" t="s">
+        <v>72</v>
+      </c>
+      <c r="F16" t="s">
         <v>95</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="1" t="s">
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" t="s">
+        <v>71</v>
+      </c>
+      <c r="D17" t="s">
+        <v>72</v>
+      </c>
+      <c r="F17" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" t="s">
+        <v>73</v>
+      </c>
+      <c r="D18" t="s">
         <v>102</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="G18" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" t="s">
+        <v>75</v>
+      </c>
+      <c r="D19" t="s">
+        <v>74</v>
+      </c>
+      <c r="G19" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D10" s="1" t="s">
+      <c r="C20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D20" t="s">
+        <v>53</v>
+      </c>
+      <c r="I20" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" t="s">
         <v>70</v>
       </c>
-      <c r="I10" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="I11" s="1" t="s">
+      <c r="D21" t="s">
+        <v>77</v>
+      </c>
+      <c r="G21" t="s">
+        <v>131</v>
+      </c>
+      <c r="H21" t="s">
+        <v>132</v>
+      </c>
+      <c r="I21" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22" t="s">
+        <v>70</v>
+      </c>
+      <c r="D22" t="s">
+        <v>77</v>
+      </c>
+      <c r="G22" t="s">
+        <v>134</v>
+      </c>
+      <c r="H22" t="s">
+        <v>133</v>
+      </c>
+      <c r="I22" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>38</v>
+      </c>
+      <c r="C23" t="s">
+        <v>78</v>
+      </c>
+      <c r="D23" t="s">
+        <v>79</v>
+      </c>
+      <c r="G23" t="s">
+        <v>135</v>
+      </c>
+      <c r="I23" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="12" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D12" s="1" t="s">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>39</v>
+      </c>
+      <c r="C24" t="s">
+        <v>82</v>
+      </c>
+      <c r="D24" t="s">
+        <v>79</v>
+      </c>
+      <c r="G24" t="s">
+        <v>136</v>
+      </c>
+      <c r="I24" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>40</v>
+      </c>
+      <c r="C25" t="s">
+        <v>83</v>
+      </c>
+      <c r="D25" t="s">
+        <v>84</v>
+      </c>
+      <c r="G25" t="s">
+        <v>129</v>
+      </c>
+      <c r="H25" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>185</v>
+      </c>
+      <c r="B27" t="s">
+        <v>184</v>
+      </c>
+      <c r="C27" t="s">
+        <v>80</v>
+      </c>
+      <c r="D27" t="s">
         <v>103</v>
       </c>
-      <c r="G12" s="1" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D13" s="1" t="s">
+      <c r="H27" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>137</v>
+      </c>
+      <c r="B28" t="s">
+        <v>87</v>
+      </c>
+      <c r="C28" t="s">
+        <v>81</v>
+      </c>
+      <c r="D28" t="s">
         <v>103</v>
       </c>
-      <c r="G13" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="I20" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="I21" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="I22" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="G24" s="1" t="s">
+      <c r="H28" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
         <v>138</v>
       </c>
-      <c r="I24" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="D25" s="1" t="s">
+      <c r="B29" t="s">
+        <v>88</v>
+      </c>
+      <c r="C29" t="s">
+        <v>81</v>
+      </c>
+      <c r="D29" t="s">
+        <v>103</v>
+      </c>
+      <c r="H29" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
         <v>85</v>
       </c>
-      <c r="G25" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="B27" s="1" t="s">
+      <c r="C31" t="s">
         <v>86</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="H27" s="1" t="s">
+      <c r="D31" t="s">
+        <v>91</v>
+      </c>
+      <c r="G31" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="28" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="B28" s="1" t="s">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
         <v>89</v>
       </c>
-      <c r="C28" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="H28" s="1" t="s">
+      <c r="C32" t="s">
+        <v>90</v>
+      </c>
+      <c r="D32" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="H29" s="1" t="s">
+      <c r="H33" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B31" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1" t="s">
+    <row r="34" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B34" t="s">
+        <v>147</v>
+      </c>
+      <c r="G34" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B32" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="33" spans="2:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="1" t="s">
+    <row r="35" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B35" t="s">
+        <v>148</v>
+      </c>
+      <c r="G35" t="s">
         <v>146</v>
       </c>
-      <c r="H33" s="1" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="34" spans="2:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B34" s="1" t="s">
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B36" t="s">
+        <v>149</v>
+      </c>
+      <c r="G36" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B37" t="s">
         <v>150</v>
       </c>
-      <c r="G34" s="1" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="35" spans="2:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B35" s="1" t="s">
+      <c r="G37" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B38" t="s">
         <v>151</v>
       </c>
-      <c r="G35" s="1" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="36" spans="2:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B36" s="1" t="s">
+      <c r="G38" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B39" t="s">
         <v>152</v>
       </c>
-      <c r="G36" s="1" t="s">
+      <c r="G39" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="37" spans="2:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B37" s="1" t="s">
+    <row r="40" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B40" t="s">
         <v>153</v>
       </c>
-      <c r="G37" s="1" t="s">
+      <c r="G40" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="38" spans="2:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B38" s="1" t="s">
+    <row r="41" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B41" t="s">
         <v>154</v>
       </c>
-      <c r="G38" s="1" t="s">
+      <c r="G41" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="39" spans="2:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B39" s="1" t="s">
+    <row r="42" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B42" t="s">
         <v>155</v>
       </c>
-      <c r="G39" s="1" t="s">
+      <c r="G42" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="40" spans="2:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B40" s="1" t="s">
+    <row r="43" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B43" t="s">
         <v>156</v>
       </c>
-      <c r="G40" s="1" t="s">
+      <c r="G43" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="41" spans="2:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B41" s="1" t="s">
+    <row r="44" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B44" t="s">
         <v>157</v>
       </c>
-      <c r="G41" s="1" t="s">
+      <c r="G44" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="42" spans="2:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B42" s="1" t="s">
+    <row r="45" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B45" t="s">
         <v>158</v>
       </c>
-      <c r="G42" s="1" t="s">
+      <c r="G45" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B43" s="1" t="s">
+    <row r="46" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B46" t="s">
         <v>159</v>
       </c>
-      <c r="G43" s="1" t="s">
+      <c r="G46" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B44" s="1" t="s">
+    <row r="47" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B47" t="s">
         <v>160</v>
       </c>
-      <c r="G44" s="1" t="s">
+      <c r="G47" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B45" s="1" t="s">
+    <row r="48" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B48" t="s">
         <v>161</v>
       </c>
-      <c r="G45" s="1" t="s">
+      <c r="G48" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="46" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B46" s="1" t="s">
+    <row r="49" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B49" t="s">
         <v>162</v>
       </c>
-      <c r="G46" s="1" t="s">
+      <c r="G49" t="s">
         <v>176</v>
-      </c>
-    </row>
-    <row r="47" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B47" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="G47" s="1" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="48" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B48" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="G48" s="1" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="49" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B49" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="G49" s="1" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="51" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B51" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="G51" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="52" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B52" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="G52" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="53" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="G53" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
   </sheetData>

</xml_diff>